<commit_message>
added comments and updated the paper based on reviewer feedback
</commit_message>
<xml_diff>
--- a/Journal Paper/revision/Reviewer Comments.xlsx
+++ b/Journal Paper/revision/Reviewer Comments.xlsx
@@ -122,7 +122,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="106">
   <si>
     <t>Reviewer</t>
   </si>
@@ -608,7 +608,16 @@
     <t>Danny will document the potential normalization of Kc.</t>
   </si>
   <si>
-    <t>Danny</t>
+    <t>Crop evapotranspiration is calculated based on an evapotranspiration reference surface and an endogenous or exogenous (user-defined) crop coefficient. The reference surface evapotranspiration is calculated using the daily time step method outlined in Chapter 4 of FAO paper number 56. (27)  The crop coefficient (Kc) in our model can be either exogenous or calculated endogenously. The illustrative results presented in this paper are based on the endogenous calculation of Kc. For the endogenous crop coefficient calculation, the model uses the single crop coefficient approach as outlined in Chapter 6 of FAO paper number 56.(27)  In our model, the Kc curve is constructed to reflect various wetting events, variable growing seasons (spring-summer rotations, winter rotations, and perennial crops), and variable soil textures.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kc represents a crop based constant that varies throughout the growing season, refer to FAO paper 56(27) for common ranges observed across a number of crops </t>
+  </si>
+  <si>
+    <t>The “product-purpose” allocation approach is used in our model with regard to attributing a given water footprint to an agricultural crop/product. For example, the water footprint attributed to growing corn grain is fully attributed the corn grain. However, if one were to include the harvest of corn grain and corn stover, the water footprint could be easily be allocated among the respective harvested portions of the crop using any number of user-defined allocation methods.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Crop evapotranspiration is calculated based on an evapotranspiration reference surface (i.e., the ET of a natural ecosystem) and an endogenous or exogenous (user-defined) crop coefficient. The reference surface evapotranspiration is calculated using the daily time step method outlined in Chapter 4 of FAO paper number 56. (27)  </t>
   </si>
 </sst>
 </file>
@@ -1105,10 +1114,10 @@
   <dimension ref="A1:J29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="D24" activePane="bottomRight" state="frozenSplit"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="E24" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="I29" sqref="I29"/>
+      <selection pane="bottomRight" activeCell="H37" sqref="H36:H37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1688,7 +1697,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="150" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" ht="195" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>32</v>
       </c>
@@ -1739,7 +1748,7 @@
         <v>101</v>
       </c>
       <c r="I24" s="13" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="90" x14ac:dyDescent="0.25">
@@ -1794,7 +1803,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="27" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" ht="105" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>32</v>
       </c>
@@ -1818,7 +1827,7 @@
         <v>94</v>
       </c>
       <c r="I27" s="13" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
     </row>
     <row r="28" spans="1:10" ht="165" x14ac:dyDescent="0.25">
@@ -1848,7 +1857,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="29" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>32</v>
       </c>
@@ -1872,7 +1881,7 @@
         <v>75</v>
       </c>
       <c r="I29" s="13" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Paper and Review Comment Update and Revisions
Incorporates Danny and Dana's comments
</commit_message>
<xml_diff>
--- a/Journal Paper/revision/Reviewer Comments.xlsx
+++ b/Journal Paper/revision/Reviewer Comments.xlsx
@@ -4,125 +4,19 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="210" windowWidth="23880" windowHeight="9915"/>
+    <workbookView xWindow="75" yWindow="0" windowWidth="11925" windowHeight="12165"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="145621" iterate="1" iterateDelta="1.0000000000000001E-5"/>
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
-    <author>NREL</author>
-  </authors>
-  <commentList>
-    <comment ref="I10" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>NREL:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-Dana, can you answer this?</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="I15" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>NREL:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Dana can you check in to this?</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="I19" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>NREL:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-dana, can you verify that the yield data are from statsgo? </t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="I20" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>NREL:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-I will meet with dana go go over this. I will add text describing the data extent</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="98">
   <si>
     <t>Reviewer</t>
   </si>
@@ -302,19 +196,9 @@
     <t>Official Response to the Reviewer</t>
   </si>
   <si>
-    <t>More clearly state the paper's purposed and utility.</t>
-  </si>
-  <si>
-    <t>Add text explaining data geographic resolution and modifications to alternative resolution.</t>
-  </si>
-  <si>
     <t>1. Ethan will provide Danny/Dana data from the literature review.
 2. Danny/Dana will produce better figures. Comparison of ANL (box plot), NREL (box plot), and high/low values from the literature.
 3. Ethan will revise the results text accordingly.</t>
-  </si>
-  <si>
-    <t>1. Add text explaining the missing data.
-2. Add theoretical results for missing regions.</t>
   </si>
   <si>
     <t>Better emphasize:
@@ -323,9 +207,6 @@
 3. Emphasize "proof of concept"</t>
   </si>
   <si>
-    <t>Danny/Dana will revise text describing and documenting yields</t>
-  </si>
-  <si>
     <t>Partially Accepted</t>
   </si>
   <si>
@@ -342,10 +223,6 @@
   </si>
   <si>
     <t>Reviewers said the complex or specialist terms have not been adequately explained and the innovation/advancement rated low.</t>
-  </si>
-  <si>
-    <t>1. Ethan will add text emphasizing model proof of concept and flexibility to use other yield data.
-2. Danny/Dana will revise text describing and documenting yields.</t>
   </si>
   <si>
     <t xml:space="preserve">2) Like many previous water footprint papers, the authors calculate blue water (irrigation) use as a theoretical maximum. Other authors (notably Hoekstra et al.), calculate a theoretical water requirement based on maximal yield and then derive irrigation water used by subtracting the naturally available water (precipitation or derived soil water) and assigning the deficit as a blue water footprint - whether or not irrigation is actually used. The approach was widely criticized and subsequent versions of the footprint now incorporate more realistic assumptions. This manuscript presents a similar extreme technique, with very thin justification and inadequately described methods. 
@@ -361,12 +238,6 @@
   </si>
   <si>
     <t xml:space="preserve">5) The authors may wish to consider whether both Figure 5 and 6 necessary? - Figure 6 seems to simply be an aggregate version of Figure 5. Perhaps, maps of the crop yields and total potential ET would be useful to augment the green and blue water footprints. </t>
-  </si>
-  <si>
-    <t>Respond with argument for the modeling system. Mention pre-existing NREL work on the conversion side and justify focus on the production size (i.e., geo-spatial issues).</t>
-  </si>
-  <si>
-    <t>We actually take into account a natural ecosystem. Danny/Dana will document this in the text</t>
   </si>
   <si>
     <t>We agree that it did not make sense to include both figures 5 and 6. Figure 6 has since been replaced by X. A yield figure did not seem to be appropriate since these assumptions pre-exist in the STATSGO2 and have been previously visualized. A total potential ET figure would obscure meaningful results given that we do not assume any tolerance for yield loss.</t>
@@ -384,8 +255,11 @@
 C. Wu, M., Chiu, Y., and Demissie, Y. 2012. Quantifying the Regional Water Footprint of Biofuel Using Multiple Analytical Tools, Water Resource Research. VOL. 48, W10518.</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">This section only reviewed one method – Penman-Monteith. </t>
+    <t>We have made sure that all mentions of the geographic level of existing water footprinting includes mentions of more recent county level studies throughout the paper.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Yes, you are correct that our original wording was not clear on </t>
     </r>
     <r>
       <rPr>
@@ -395,7 +269,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>There are several methodologies exist but not mentioned.</t>
+      <t>X</t>
     </r>
     <r>
       <rPr>
@@ -405,24 +279,15 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> For the models, WETT is soil erosion model and there are other models of this type. An online water footprint model WATER (http://water.es.anl.gov/) is another example of the models.</t>
-    </r>
-  </si>
-  <si>
-    <t>Dana</t>
-  </si>
-  <si>
-    <t>Section 2 is intended to focus soly on methods and models related to a complete water footprinting and not partial footprints or other related issues such as water quality or soil erosian. We mention the WEPP model as an example of other water related models that we are not covering in detail. We added text to make this clearer. We also added text and a link to ANL's model.</t>
-  </si>
-  <si>
-    <t>As suggested this recent literature has been added to the paper in sectio n2</t>
-  </si>
-  <si>
-    <t>We have made sure that all mentions of the geographic level of existing water footprinting includes mentions of more recent county level studies throughout the paper.</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Yes, you are correct that our original wording was not clear on </t>
+      <t>. We have rewriten this sentence to essentially state the importance of consistent multi-crop comparisons under alternative conditions/assumptions.</t>
+    </r>
+  </si>
+  <si>
+    <t>We made the suggested correction.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">We used the single crop coefficient method as outlined in FAO paper 56 for each crop assessed. We have added clarifying language around this to the paper on </t>
     </r>
     <r>
       <rPr>
@@ -437,126 +302,64 @@
     <r>
       <rPr>
         <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Language has been clarified to indicate that the P-M equation is calculated daily on </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>X</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">As suggested we added a more succinct verification analysis of green water by illustrating literature results alongside our own results. These results are shown in Figure </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>X</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>. We have rewriten this sentence to essentially state the importance of consistent multi-crop comparisons under alternative conditions/assumptions.</t>
-    </r>
-  </si>
-  <si>
-    <t>We made the suggested correction.</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">We used the single crop coefficient method as outlined in FAO paper 56 for each crop assessed. We have added clarifying language around this to the paper on </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>X</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
       <t>.</t>
     </r>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">As suggested we more clearly an concisely state the limitations of the existing literature and the novelty of our paper in the abstract and </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>X</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Language has been clarified to indicate that the P-M equation is calculated daily on </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>X</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">As suggested we added a more succinct verification analysis of green water by illustrating literature results alongside our own results. These results are shown in Figure </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>X</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.</t>
-    </r>
-  </si>
-  <si>
     <t>As suggested the results and conclusion sections were trimmed down to essential information.</t>
-  </si>
-  <si>
-    <t>Thank you for your comments. The contribution of our modeling system should now be more clearly and concisely stated in the abstract as well as X.</t>
-  </si>
-  <si>
-    <t>It should be noted that the blue water foot print, as calculated in this model, is affected by an assumed tolerance to crop yield loss. For purposes of illustration, we have assumed this parameter to be zero; in other words we assume that there is no tolerance to yield reduction and thus the blue water values reported should be viewed as maxima. In practice, however, there will be some level of tolerance to yield loss. As opposed to a yield maximizing model, which is our default case, the model could be easily modified to be water maximizing with the appropriate data.</t>
-  </si>
-  <si>
-    <t>Danny/Dana need to address this since I actually don't understand how the model handles this either.</t>
   </si>
   <si>
     <t>x</t>
@@ -586,9 +389,6 @@
       <t>.
 With regards to journal appropriateness, feedstock focused studies appear to fall into the scope of Biofpr journal articles (http://onlinelibrary.wiley.com/journal/10.1002/(ISSN)1932-1031/homepage/ProductInformation.html).</t>
     </r>
-  </si>
-  <si>
-    <t>Danny: Danny your previous comment here does not actually address any of the issues in this reviewer's comment.</t>
   </si>
   <si>
     <t>1. Ethan will provide Danny/Dana data from the literature review.
@@ -602,29 +402,288 @@
 </t>
   </si>
   <si>
-    <t>Danny will document Kc calculations.</t>
-  </si>
-  <si>
-    <t>Danny will document the potential normalization of Kc.</t>
-  </si>
-  <si>
-    <t>Crop evapotranspiration is calculated based on an evapotranspiration reference surface and an endogenous or exogenous (user-defined) crop coefficient. The reference surface evapotranspiration is calculated using the daily time step method outlined in Chapter 4 of FAO paper number 56. (27)  The crop coefficient (Kc) in our model can be either exogenous or calculated endogenously. The illustrative results presented in this paper are based on the endogenous calculation of Kc. For the endogenous crop coefficient calculation, the model uses the single crop coefficient approach as outlined in Chapter 6 of FAO paper number 56.(27)  In our model, the Kc curve is constructed to reflect various wetting events, variable growing seasons (spring-summer rotations, winter rotations, and perennial crops), and variable soil textures.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kc represents a crop based constant that varies throughout the growing season, refer to FAO paper 56(27) for common ranges observed across a number of crops </t>
-  </si>
-  <si>
-    <t>The “product-purpose” allocation approach is used in our model with regard to attributing a given water footprint to an agricultural crop/product. For example, the water footprint attributed to growing corn grain is fully attributed the corn grain. However, if one were to include the harvest of corn grain and corn stover, the water footprint could be easily be allocated among the respective harvested portions of the crop using any number of user-defined allocation methods.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Crop evapotranspiration is calculated based on an evapotranspiration reference surface (i.e., the ET of a natural ecosystem) and an endogenous or exogenous (user-defined) crop coefficient. The reference surface evapotranspiration is calculated using the daily time step method outlined in Chapter 4 of FAO paper number 56. (27)  </t>
+    <r>
+      <t xml:space="preserve">This section only reviewed one method – Penman-Monteith. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">There are several methodologies exist but not mentioned. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>For the models, WETT is soil erosion model and there are other models of this type. An online water footprint model WATER (http://water.es.anl.gov/) is another example of the models.</t>
+    </r>
+  </si>
+  <si>
+    <t>As suggested this recent literature has been added to the paper in section 2</t>
+  </si>
+  <si>
+    <t>Section 2 is intended to focus soly on methods and models related to a complete water footprinting and not partial footprints or other related issues such as water quality or soil erosian. We mention the WEPP model as an example of other water related models that we are not covering in detail. We added text to make this clearer in section 2. We also added text and a link to ANL's model.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Our method is now more clearly described on </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>X</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">. Map unit composition was determined by transecting or sampling areas on the more detailed maps and then statistically expanding the data to characterize the whole map unit. " http://www.nrcs.usda.gov/wps/portal/nrcs/detail/soils/home/?cid=nrcs142p2_053629. The spatial dataset is distributed in state, territorial, and national extents, we used the soil mapping unit at the national extents level. </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Geographic coverage is limited to the available data as better described on </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>X</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">. The underlying SSURGO tablular data used in relationship with the STATSGO mapping unit data contains soil property and crop yield data used in the model. The non-irrigated yields for corn and soybeans from SSURGO were aggregated to the soil mapping units resulting in the geographic coverage in the figures. </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Thank you for your comments. The contribution of our modeling system should now be more clearly and concisely stated in the abstract as well as  throughout the paper (e.g., </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>X</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>).</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">As suggested we more clearly an concisely state the limitations of the existing literature and the novelty of our paper in the abstract and throughout the paper (e.g., </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>X</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>).</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">The non-irrigated yields from the SSURGO tablular data were used in the model in relationship to the STATSGO soil mapping units. 
+Soil Survey Staff, Natural Resources Conservation Service, United States Department of Agriculture. Web Soil Survey. Available online at http://websoilsurvey.nrcs.usda.gov/. SSURGOV2.1
+MD 2.2.5. This is more clearly documented on </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>X</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">See additional metadata &amp; figure on X. The crop yields were queried from the Access database "tabular SSURGO" portion of the NRCS download. The crop yields were aggregated to the STATSGO soil mapping units (Musym). The determinate for the individual crop geographic coverage in the model was the layering of the data from different sources. The data model pares locations where data is missing  or NULL along the query chain. Several sources were used to fill in the planting and harvesting crop dates at the top layer. In addition, the model is structured such that other sources of the climate and soil data , including yield, could be substituted as exogenous inputs. </t>
+  </si>
+  <si>
+    <r>
+      <t>We address these issues more thoroughly here on</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> X</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>. It should be noted that the blue water foot print, as calculated in this model, is affected by an assumed tolerance to crop yield loss. For purposes of illustration, we have assumed this parameter to be zero; in other words we assume that there is no tolerance to yield reduction and thus the blue water values reported should be viewed as maxima. In practice, however, there will be some level of tolerance to yield loss. As opposed to a yield maximizing model, which is our default case, the model could be easily modified to be water maximizing with the appropriate data.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Additional description of our methods addressing this are included on </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>X</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>. Crop evapotranspiration is calculated based on an evapotranspiration reference surface (i.e., the ET of a natural ecosystem) and an endogenous or exogenous (user-defined) crop coefficient. The reference surface evapotranspiration is calculated using the daily time step method outlined in Chapter 4 of FAO paper number 56.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Additional description of our methods addressing this are included on </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>X</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>. The “product-purpose” allocation approach is used in our model with regard to attributing a given water footprint to an agricultural crop/product. For example, the water footprint attributed to growing corn grain is fully attributed the corn grain. However, if one were to include the harvest of corn grain and corn stover, the water footprint could be easily be allocated among the respective harvested portions of the crop using any number of user-defined allocation methods.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Additional description of our methods addressing this are included on </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>X</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">. Kc represents a crop based constant that varies throughout the growing season, refer to FAO paper 56 for common ranges observed across a number of crops </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Additional description of our methods addressing this are included on </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>X</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>. Crop evapotranspiration is calculated based on an evapotranspiration reference surface and an endogenous or exogenous (user-defined) crop coefficient. The reference surface evapotranspiration is calculated using the daily time step method outlined in Chapter 4 of FAO paper number 56. The crop coefficient (Kc) in our model can be either exogenous or calculated endogenously. The illustrative results presented in this paper are based on the endogenous calculation of Kc. For the endogenous crop coefficient calculation, the model uses the single crop coefficient approach as outlined in Chapter 6 of FAO paper number 56. In our model, the Kc curve is constructed to reflect various wetting events, variable growing seasons (spring-summer rotations, winter rotations, and perennial crops), and variable soil textures.</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -638,40 +697,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -750,7 +775,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -786,19 +811,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1110,14 +1129,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="E24" activePane="bottomRight" state="frozenSplit"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="D25" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="H37" sqref="H36:H37"/>
+      <selection pane="bottomRight" activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1139,11 +1158,11 @@
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
-      <c r="E1" s="19" t="s">
+      <c r="E1" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
       <c r="H1" s="8"/>
       <c r="I1" s="1"/>
     </row>
@@ -1217,7 +1236,7 @@
       <c r="G4" s="3"/>
       <c r="H4" s="5"/>
       <c r="I4" s="2" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="90" x14ac:dyDescent="0.25">
@@ -1228,9 +1247,9 @@
         <v>13</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="D5" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="D5" s="11" t="s">
         <v>55</v>
       </c>
       <c r="E5" s="3" t="s">
@@ -1242,7 +1261,7 @@
       <c r="G5" s="3"/>
       <c r="H5" s="5"/>
       <c r="I5" s="2" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="120" x14ac:dyDescent="0.25">
@@ -1253,7 +1272,7 @@
         <v>13</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="D6" s="11" t="s">
         <v>54</v>
@@ -1267,7 +1286,7 @@
       <c r="G6" s="3"/>
       <c r="H6" s="5"/>
       <c r="I6" s="2" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -1292,7 +1311,7 @@
       <c r="G7" s="3"/>
       <c r="H7" s="5"/>
       <c r="I7" s="2" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1317,7 +1336,7 @@
       <c r="G8" s="3"/>
       <c r="H8" s="5"/>
       <c r="I8" s="2" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="196.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1340,14 +1359,12 @@
         <v>42</v>
       </c>
       <c r="G9" s="3"/>
-      <c r="H9" s="5" t="s">
-        <v>57</v>
-      </c>
+      <c r="H9" s="5"/>
       <c r="I9" s="2" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="120" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>5</v>
       </c>
@@ -1357,7 +1374,7 @@
       <c r="C10" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D10" s="16" t="s">
+      <c r="D10" s="11" t="s">
         <v>54</v>
       </c>
       <c r="E10" s="3" t="s">
@@ -1367,11 +1384,9 @@
       <c r="G10" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="H10" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="I10" s="14" t="s">
-        <v>81</v>
+      <c r="H10" s="5"/>
+      <c r="I10" s="15" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -1396,7 +1411,7 @@
       <c r="G11" s="3"/>
       <c r="H11" s="5"/>
       <c r="I11" s="2" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="60" x14ac:dyDescent="0.25">
@@ -1420,8 +1435,8 @@
         <v>42</v>
       </c>
       <c r="H12" s="5"/>
-      <c r="I12" s="17" t="s">
-        <v>87</v>
+      <c r="I12" s="15" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -1445,8 +1460,8 @@
         <v>42</v>
       </c>
       <c r="H13" s="5"/>
-      <c r="I13" s="17" t="s">
-        <v>89</v>
+      <c r="I13" s="15" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="90" x14ac:dyDescent="0.25">
@@ -1457,9 +1472,9 @@
         <v>26</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="D14" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="D14" s="14" t="s">
         <v>54</v>
       </c>
       <c r="E14" s="3" t="s">
@@ -1472,13 +1487,13 @@
         <v>42</v>
       </c>
       <c r="H14" s="5" t="s">
-        <v>98</v>
+        <v>82</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>5</v>
       </c>
@@ -1488,7 +1503,7 @@
       <c r="C15" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D15" s="16" t="s">
+      <c r="D15" s="11" t="s">
         <v>54</v>
       </c>
       <c r="E15" s="3" t="s">
@@ -1498,11 +1513,9 @@
       <c r="G15" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="H15" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="I15" s="14" t="s">
-        <v>81</v>
+      <c r="H15" s="5"/>
+      <c r="I15" s="15" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -1527,7 +1540,7 @@
       <c r="G16" s="3"/>
       <c r="H16" s="5"/>
       <c r="I16" s="2" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -1535,12 +1548,12 @@
         <v>32</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="D17" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="D17" s="13" t="s">
         <v>54</v>
       </c>
       <c r="E17" s="3" t="s">
@@ -1551,7 +1564,7 @@
       </c>
       <c r="G17" s="3"/>
       <c r="H17" s="5" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="I17" s="2" t="s">
         <v>4</v>
@@ -1579,10 +1592,10 @@
       <c r="G18" s="3"/>
       <c r="H18" s="5"/>
       <c r="I18" s="2" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>32</v>
       </c>
@@ -1592,7 +1605,7 @@
       <c r="C19" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D19" s="16" t="s">
+      <c r="D19" s="11" t="s">
         <v>55</v>
       </c>
       <c r="E19" s="3" t="s">
@@ -1604,14 +1617,12 @@
       <c r="G19" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="H19" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="I19" s="14" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" ht="150" x14ac:dyDescent="0.25">
+      <c r="H19" s="5"/>
+      <c r="I19" s="15" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="165" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>32</v>
       </c>
@@ -1621,7 +1632,7 @@
       <c r="C20" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="D20" s="16" t="s">
+      <c r="D20" s="11" t="s">
         <v>55</v>
       </c>
       <c r="E20" s="3" t="s">
@@ -1631,14 +1642,12 @@
       <c r="G20" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="H20" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="I20" s="14" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" ht="315" x14ac:dyDescent="0.25">
+      <c r="H20" s="5"/>
+      <c r="I20" s="15" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="270" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>32</v>
       </c>
@@ -1646,10 +1655,10 @@
         <v>32</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="D21" s="16" t="s">
-        <v>63</v>
+        <v>65</v>
+      </c>
+      <c r="D21" s="13" t="s">
+        <v>59</v>
       </c>
       <c r="E21" s="3" t="s">
         <v>45</v>
@@ -1659,14 +1668,12 @@
         <v>42</v>
       </c>
       <c r="H21" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="I21" s="13" t="s">
-        <v>97</v>
-      </c>
-      <c r="J21" s="18" t="s">
+        <v>83</v>
+      </c>
+      <c r="I21" s="15" t="s">
         <v>93</v>
       </c>
+      <c r="J21" s="16"/>
     </row>
     <row r="22" spans="1:10" ht="216.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
@@ -1676,10 +1683,10 @@
         <v>33</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="D22" s="16" t="s">
-        <v>64</v>
+        <v>66</v>
+      </c>
+      <c r="D22" s="14" t="s">
+        <v>60</v>
       </c>
       <c r="E22" s="3" t="s">
         <v>45</v>
@@ -1691,13 +1698,13 @@
         <v>42</v>
       </c>
       <c r="H22" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="I22" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="195" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" ht="210" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>32</v>
       </c>
@@ -1707,8 +1714,8 @@
       <c r="C23" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="D23" s="16" t="s">
-        <v>64</v>
+      <c r="D23" s="11" t="s">
+        <v>60</v>
       </c>
       <c r="E23" s="3" t="s">
         <v>45</v>
@@ -1717,14 +1724,12 @@
       <c r="G23" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="H23" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="I23" s="13" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="H23" s="5"/>
+      <c r="I23" s="15" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>32</v>
       </c>
@@ -1732,10 +1737,10 @@
         <v>35</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="D24" s="16" t="s">
-        <v>64</v>
+        <v>67</v>
+      </c>
+      <c r="D24" s="11" t="s">
+        <v>60</v>
       </c>
       <c r="E24" s="3" t="s">
         <v>44</v>
@@ -1744,11 +1749,9 @@
       <c r="G24" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="H24" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="I24" s="13" t="s">
-        <v>103</v>
+      <c r="H24" s="5"/>
+      <c r="I24" s="15" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="90" x14ac:dyDescent="0.25">
@@ -1759,10 +1762,10 @@
         <v>36</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="D25" s="11" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="E25" s="3" t="s">
         <v>44</v>
@@ -1775,7 +1778,7 @@
       </c>
       <c r="H25" s="5"/>
       <c r="I25" s="2" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
@@ -1789,7 +1792,7 @@
         <v>48</v>
       </c>
       <c r="D26" s="11" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="E26" s="3" t="s">
         <v>44</v>
@@ -1800,10 +1803,10 @@
       <c r="G26" s="3"/>
       <c r="H26" s="5"/>
       <c r="I26" s="2" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" ht="105" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" ht="120" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>32</v>
       </c>
@@ -1813,21 +1816,19 @@
       <c r="C27" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="D27" s="16" t="s">
-        <v>64</v>
+      <c r="D27" s="11" t="s">
+        <v>60</v>
       </c>
       <c r="E27" s="3" t="s">
         <v>44</v>
       </c>
       <c r="F27" s="3"/>
       <c r="G27" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="H27" s="5"/>
+      <c r="I27" s="15" t="s">
         <v>95</v>
-      </c>
-      <c r="H27" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="I27" s="13" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="28" spans="1:10" ht="165" x14ac:dyDescent="0.25">
@@ -1841,7 +1842,7 @@
         <v>50</v>
       </c>
       <c r="D28" s="11" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="E28" s="3" t="s">
         <v>44</v>
@@ -1850,14 +1851,12 @@
         <v>42</v>
       </c>
       <c r="G28" s="3"/>
-      <c r="H28" s="5" t="s">
-        <v>74</v>
-      </c>
+      <c r="H28" s="5"/>
       <c r="I28" s="2" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" ht="105" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>32</v>
       </c>
@@ -1867,8 +1866,8 @@
       <c r="C29" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="D29" s="16" t="s">
-        <v>64</v>
+      <c r="D29" s="11" t="s">
+        <v>60</v>
       </c>
       <c r="E29" s="3" t="s">
         <v>43</v>
@@ -1877,11 +1876,9 @@
       <c r="G29" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="H29" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="I29" s="13" t="s">
-        <v>105</v>
+      <c r="H29" s="5"/>
+      <c r="I29" s="15" t="s">
+        <v>94</v>
       </c>
     </row>
   </sheetData>
@@ -1890,7 +1887,6 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>